<commit_message>
Chrome driver config update
</commit_message>
<xml_diff>
--- a/TestSteps.xlsx
+++ b/TestSteps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sensa NR\2024\AI_Selenium\AI_SNR_Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D2F6F64-AD50-4948-B2CF-12591B10EFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20220CE-9B88-4098-8223-34E35C36177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{C27EA07C-E797-433D-A02A-B0B12C84BE2E}"/>
   </bookViews>
@@ -41,10 +41,10 @@
     <t>Visit https://magento.softwaretestingboard.com/</t>
   </si>
   <si>
-    <t>Click mens &gt; tops &gt; tees</t>
+    <t>Select 1 product and add to cart</t>
   </si>
   <si>
-    <t>Select 1 product and add to cart</t>
+    <t>Click mens &gt; tops &gt; tee</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -434,12 +434,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>